<commit_message>
Módulo 05 - finalização
</commit_message>
<xml_diff>
--- a/módulo 05/aula-formulas-matematica.xlsx
+++ b/módulo 05/aula-formulas-matematica.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Google Drive\Curso_Excel\05 Primeiras fórmulas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Curso Excel do básico ao avançado\módulo 05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B50DD66-6FCD-44F2-A819-E7A6D62CD11B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{9677FD8D-6660-41E5-9A81-FFEA2AD51EE9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8670" windowHeight="6780" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="8" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="Cad_Motorista" sheetId="11" r:id="rId4"/>
     <sheet name="Ind_Km_Veículos" sheetId="12" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
   <si>
     <t>EMPRESA</t>
   </si>
@@ -238,11 +237,17 @@
     <t>Número de Veículos
 da Frota</t>
   </si>
+  <si>
+    <t>Conta valores/células sem valores vazios</t>
+  </si>
+  <si>
+    <t>Conta valores númericos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="\(##\)\ 0\ 0000&quot;-&quot;0000"/>
@@ -320,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -409,9 +414,6 @@
     <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -422,6 +424,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -487,7 +495,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6BA0FC6-3102-4105-B76E-A3425C0258A0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B6BA0FC6-3102-4105-B76E-A3425C0258A0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -570,7 +578,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F412B0-641D-4F8B-B908-24115BAD6C2C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{29F412B0-641D-4F8B-B908-24115BAD6C2C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -690,7 +698,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCF631DB-37CE-486B-B435-8473605BF212}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DCF631DB-37CE-486B-B435-8473605BF212}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -771,7 +779,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C08429E-7AEF-47DA-9312-B3EFFFD47D63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C08429E-7AEF-47DA-9312-B3EFFFD47D63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -853,7 +861,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEB3F770-62EA-44CF-A1B6-CBDB1F0154E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EEB3F770-62EA-44CF-A1B6-CBDB1F0154E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -934,7 +942,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2899AFD7-F534-4291-A4B0-8AAF42D3C45B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2899AFD7-F534-4291-A4B0-8AAF42D3C45B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1018,7 +1026,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3627734-0663-4FA9-8780-F55E760F1049}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3627734-0663-4FA9-8780-F55E760F1049}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1099,7 +1107,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC11C314-5AC1-4502-847C-2E61C5CAC00B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FC11C314-5AC1-4502-847C-2E61C5CAC00B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1219,7 +1227,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A018AF23-8EA1-4733-ADD0-8BD8E14326F9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A018AF23-8EA1-4733-ADD0-8BD8E14326F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1302,7 +1310,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B68638E9-237B-4AB4-BD76-E5FF66A2646F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B68638E9-237B-4AB4-BD76-E5FF66A2646F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1384,7 +1392,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78A4E03F-FBDB-42CE-9CEF-F8500D7571E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{78A4E03F-FBDB-42CE-9CEF-F8500D7571E9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1465,7 +1473,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C2157E-B594-4473-AB0A-20088837B6C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8C2157E-B594-4473-AB0A-20088837B6C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1544,7 +1552,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0024708-7F6B-4F06-A977-802C798E7611}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0024708-7F6B-4F06-A977-802C798E7611}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1626,7 +1634,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F871882-370C-4E6B-9ED5-6934223D9A2A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8F871882-370C-4E6B-9ED5-6934223D9A2A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1714,7 +1722,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A64CEA9A-4C88-4133-9DF5-BE5DB64BED22}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A64CEA9A-4C88-4133-9DF5-BE5DB64BED22}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1807,7 +1815,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F2EF660-7474-4CD1-B077-0422EA1DE591}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4F2EF660-7474-4CD1-B077-0422EA1DE591}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1888,7 +1896,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16FDE091-B1C0-4486-BEC7-834E97580F0C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{16FDE091-B1C0-4486-BEC7-834E97580F0C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2008,7 +2016,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C29C9295-0E79-43A4-A139-C0D744B4C204}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C29C9295-0E79-43A4-A139-C0D744B4C204}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2091,7 +2099,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C5A30B4-9A56-48C5-A173-5F0E10A7AB7E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7C5A30B4-9A56-48C5-A173-5F0E10A7AB7E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2173,7 +2181,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D12ED82-1966-40CD-9E3C-05EF439074E8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6D12ED82-1966-40CD-9E3C-05EF439074E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2254,7 +2262,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E0851EE-3980-4CF3-9523-FD6F20A09F57}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3E0851EE-3980-4CF3-9523-FD6F20A09F57}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2333,7 +2341,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00BE3D7A-4446-4BEA-A7CB-DB25B6586066}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00BE3D7A-4446-4BEA-A7CB-DB25B6586066}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2421,7 +2429,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB659196-ECF7-4D92-8830-DC4A35CF8B23}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CB659196-ECF7-4D92-8830-DC4A35CF8B23}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2503,7 +2511,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1765B02A-B454-4EB9-8653-55C085C8D0BB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1765B02A-B454-4EB9-8653-55C085C8D0BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2596,7 +2604,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{687357EC-8C7C-41E6-BC98-40CF0DB7E1CC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{687357EC-8C7C-41E6-BC98-40CF0DB7E1CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2677,7 +2685,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E273CD41-0863-4D4B-AD5E-C2F31D84A70C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E273CD41-0863-4D4B-AD5E-C2F31D84A70C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2797,7 +2805,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DE7789A-574B-4EF5-AC20-13EE21124EE6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6DE7789A-574B-4EF5-AC20-13EE21124EE6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2880,7 +2888,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B93ABDEB-7E13-4C91-95D9-9FB5F6B1CC79}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B93ABDEB-7E13-4C91-95D9-9FB5F6B1CC79}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2962,7 +2970,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB22967A-FF0E-4073-8C69-74EF7F36C182}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AB22967A-FF0E-4073-8C69-74EF7F36C182}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3043,7 +3051,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{875BB76A-28F7-4C24-9428-5CF75AB39CDC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{875BB76A-28F7-4C24-9428-5CF75AB39CDC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3122,7 +3130,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AA0C125-7FA2-42DD-A022-E130DCF31A2C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4AA0C125-7FA2-42DD-A022-E130DCF31A2C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3210,7 +3218,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8ED9A2C-2351-485B-BE55-EACC611E479D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8ED9A2C-2351-485B-BE55-EACC611E479D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3298,7 +3306,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EC9340D-B862-4EFA-A6D8-EE3E27D0E02F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3EC9340D-B862-4EFA-A6D8-EE3E27D0E02F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3385,7 +3393,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51B32614-DFA8-4D74-A7E8-92EE28F31ED9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{51B32614-DFA8-4D74-A7E8-92EE28F31ED9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3466,7 +3474,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6D34DA7-6AF5-4A26-B98B-8C901D0AB1BF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A6D34DA7-6AF5-4A26-B98B-8C901D0AB1BF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3586,7 +3594,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE84E718-ADF1-4D17-8876-F781156FCF2E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE84E718-ADF1-4D17-8876-F781156FCF2E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3667,7 +3675,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49F6181B-EB5B-4857-8025-EBD7CE8C2552}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{49F6181B-EB5B-4857-8025-EBD7CE8C2552}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3749,7 +3757,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2A7E9C4-0C14-4286-88D6-C53F97D16949}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C2A7E9C4-0C14-4286-88D6-C53F97D16949}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3832,7 +3840,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E167F8BE-E0B3-46B8-8155-BB827D604551}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E167F8BE-E0B3-46B8-8155-BB827D604551}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3911,7 +3919,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F90018C-C134-4F60-A6FE-F3BBD5587D70}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9F90018C-C134-4F60-A6FE-F3BBD5587D70}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3992,7 +4000,7 @@
         <xdr:cNvPr id="9" name="Retângulo: Cantos Superiores Recortados 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DE96387-781A-4BF4-A11E-E6CB028E5A6B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1DE96387-781A-4BF4-A11E-E6CB028E5A6B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4079,7 +4087,7 @@
         <xdr:cNvPr id="10" name="Retângulo: Cantos Superiores Recortados 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADB96F24-1344-4775-91F6-5799ECAE190E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ADB96F24-1344-4775-91F6-5799ECAE190E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4447,10 +4455,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46F83BD-F3BF-43E4-9A28-8E259EC6705F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
@@ -4529,12 +4537,12 @@
       </c>
     </row>
     <row r="25" spans="13:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M25" s="35">
+      <c r="M25" s="34">
         <f ca="1">TODAY()</f>
-        <v>43410</v>
-      </c>
-      <c r="N25" s="35"/>
-      <c r="O25" s="35"/>
+        <v>45352</v>
+      </c>
+      <c r="N25" s="34"/>
+      <c r="O25" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4547,7 +4555,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F21D338-352F-44D6-9932-736A440D777F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4666,7 +4674,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{596A196C-9CE3-40B9-AE7D-0ADEF9C03F4E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4783,7 +4791,7 @@
       </c>
       <c r="I5" s="16">
         <f ca="1">(TODAY()-G5)/365</f>
-        <v>5.0712328767123287</v>
+        <v>10.391780821917807</v>
       </c>
       <c r="J5" s="17">
         <f>YEAR(G5)+5</f>
@@ -4825,7 +4833,7 @@
       </c>
       <c r="I6" s="16">
         <f ca="1">(TODAY()-G6)/365</f>
-        <v>1.4438356164383561</v>
+        <v>6.7643835616438359</v>
       </c>
       <c r="J6" s="17">
         <f>YEAR(G6)+5</f>
@@ -4833,7 +4841,7 @@
       </c>
       <c r="K6" s="23" t="str">
         <f ca="1">IF(I6&gt;5,"Alta","Baixa")</f>
-        <v>Baixa</v>
+        <v>Alta</v>
       </c>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
@@ -4867,7 +4875,7 @@
       </c>
       <c r="I7" s="16">
         <f ca="1">(TODAY()-G7)/365</f>
-        <v>3.3232876712328765</v>
+        <v>8.6438356164383556</v>
       </c>
       <c r="J7" s="17">
         <f>YEAR(G7)+5</f>
@@ -4875,7 +4883,7 @@
       </c>
       <c r="K7" s="23" t="str">
         <f ca="1">IF(I7&gt;5,"Alta","Baixa")</f>
-        <v>Baixa</v>
+        <v>Alta</v>
       </c>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
@@ -5467,10 +5475,10 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Tipo de combustível inválido!" error="Selecione um dos tipos de combustível disponíveis." sqref="E5:E31" xr:uid="{EBF39E31-3EFF-452C-8162-8407A658C179}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Tipo de combustível inválido!" error="Selecione um dos tipos de combustível disponíveis." sqref="E5:E31">
       <formula1>"Diesel,Etanol,Flex,Gasolina,GNV"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Estado da compra inválido!" error="Selecione um dos tipos de estados da compra válidos." sqref="H5:H31" xr:uid="{FD2C5DED-2D25-49F7-871E-3ADDF2ABFECC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Estado da compra inválido!" error="Selecione um dos tipos de estados da compra válidos." sqref="H5:H31">
       <formula1>"Novo,Usado"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5481,7 +5489,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78E42239-30B6-4778-8F0C-BF94D02189A5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P55"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -5585,7 +5593,7 @@
       </c>
       <c r="H5" s="22" t="str">
         <f ca="1">IF(B5="","",IF(G5&gt;Início!$M$25,"OK","Vencida"))</f>
-        <v>OK</v>
+        <v>Vencida</v>
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
@@ -6378,7 +6386,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Categoria Inválida!" error="Selecione uma das categorias disponíveis." sqref="F5:F18" xr:uid="{3E89EE8C-0A27-417A-B914-72104152AA8F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Categoria Inválida!" error="Selecione uma das categorias disponíveis." sqref="F5:F18">
       <formula1>"A,B,C,D,E,AB,AC,AD,AE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6389,16 +6397,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42ABC5AE-C7C6-490C-B019-C14DA0086975}">
-  <dimension ref="A1:P58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P59"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="15" width="12.42578125" style="13" customWidth="1"/>
+    <col min="1" max="12" width="12.42578125" style="13" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" style="13" customWidth="1"/>
+    <col min="14" max="15" width="12.42578125" style="13" customWidth="1"/>
     <col min="16" max="16" width="2.28515625" style="13" hidden="1" customWidth="1"/>
     <col min="17" max="16384" width="11.7109375" style="13" hidden="1"/>
   </cols>
@@ -6441,38 +6451,78 @@
       <c r="A4" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36" t="s">
+      <c r="E4" s="35"/>
+      <c r="F4" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36" t="s">
+      <c r="G4" s="35"/>
+      <c r="H4" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="I4" s="36"/>
+      <c r="I4" s="35"/>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="28">
         <v>2018</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-    </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B5" s="36">
+        <f>N13</f>
+        <v>38414</v>
+      </c>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36">
+        <f>MAX(B9:M12)</f>
+        <v>1615</v>
+      </c>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36">
+        <f>MIN(B9:M12)</f>
+        <v>636</v>
+      </c>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36">
+        <f>COUNTA(A9:A12)</f>
+        <v>4</v>
+      </c>
+      <c r="I5" s="36"/>
+      <c r="J5" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="38">
+        <f>LARGE(B9:M12,1)</f>
+        <v>1615</v>
+      </c>
+      <c r="E6" s="38"/>
+      <c r="F6" s="37">
+        <f>SMALL(B9:M12,1)</f>
+        <v>636</v>
+      </c>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37">
+        <f>COUNT(A9:A12)</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="37"/>
+      <c r="J6" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="37">
+        <f>COUNTBLANK(A9:A12)</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="37"/>
+    </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>45</v>
@@ -6560,8 +6610,14 @@
       <c r="M9" s="29">
         <v>932</v>
       </c>
-      <c r="N9" s="30"/>
-      <c r="O9" s="34"/>
+      <c r="N9" s="30">
+        <f>SUM(B9:M9)</f>
+        <v>10499</v>
+      </c>
+      <c r="O9" s="33">
+        <f>AVERAGE(N9/12)</f>
+        <v>874.91666666666663</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -6603,106 +6659,204 @@
       <c r="M10" s="30">
         <v>1433</v>
       </c>
-      <c r="N10" s="30"/>
-      <c r="O10" s="34"/>
+      <c r="N10" s="30">
+        <f>SUM(B10:M10)</f>
+        <v>15550</v>
+      </c>
+      <c r="O10" s="33">
+        <f>AVERAGE(B10:M10)</f>
+        <v>1295.8333333333333</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="12">
+        <v>23</v>
+      </c>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="33"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="30">
+      <c r="B12" s="30">
         <v>1053</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C12" s="30">
         <v>766</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D12" s="30">
         <v>1615</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E12" s="30">
         <v>1180</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F12" s="30">
         <v>923</v>
       </c>
-      <c r="G11" s="30">
+      <c r="G12" s="30">
         <v>784</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H12" s="30">
         <v>1286</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I12" s="30">
         <v>751</v>
       </c>
-      <c r="J11" s="30">
+      <c r="J12" s="30">
         <v>1036</v>
       </c>
-      <c r="K11" s="30">
+      <c r="K12" s="30">
         <v>1011</v>
       </c>
-      <c r="L11" s="30">
+      <c r="L12" s="30">
         <v>636</v>
       </c>
-      <c r="M11" s="30">
+      <c r="M12" s="30">
         <v>1324</v>
       </c>
-      <c r="N11" s="30"/>
-      <c r="O11" s="34"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="33"/>
+      <c r="N12" s="30">
+        <f>SUM(B12:M12)</f>
+        <v>12365</v>
+      </c>
+      <c r="O12" s="33">
+        <f>AVERAGE(B12:M12)</f>
+        <v>1030.4166666666667</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="32">
+        <f>SUM(B9:B12)</f>
+        <v>3291</v>
+      </c>
+      <c r="C13" s="32">
+        <f t="shared" ref="C13:F13" si="0">SUM(C9:C12)</f>
+        <v>2793</v>
+      </c>
+      <c r="D13" s="32">
+        <f t="shared" si="0"/>
+        <v>3991</v>
+      </c>
+      <c r="E13" s="32">
+        <f t="shared" si="0"/>
+        <v>3378</v>
+      </c>
+      <c r="F13" s="32">
+        <f t="shared" si="0"/>
+        <v>3039</v>
+      </c>
+      <c r="G13" s="32">
+        <f t="shared" ref="G13" si="1">SUM(G9:G12)</f>
+        <v>2988</v>
+      </c>
+      <c r="H13" s="32">
+        <f t="shared" ref="H13" si="2">SUM(H9:H12)</f>
+        <v>3533</v>
+      </c>
+      <c r="I13" s="32">
+        <f t="shared" ref="I13:J13" si="3">SUM(I9:I12)</f>
+        <v>3150</v>
+      </c>
+      <c r="J13" s="32">
+        <f t="shared" si="3"/>
+        <v>2993</v>
+      </c>
+      <c r="K13" s="32">
+        <f t="shared" ref="K13" si="4">SUM(K9:K12)</f>
+        <v>3041</v>
+      </c>
+      <c r="L13" s="32">
+        <f t="shared" ref="L13" si="5">SUM(L9:L12)</f>
+        <v>2528</v>
+      </c>
+      <c r="M13" s="32">
+        <f>SUM(M9:M12)</f>
+        <v>3689</v>
+      </c>
+      <c r="N13" s="32">
+        <f>SUM(N9:N12)</f>
+        <v>38414</v>
+      </c>
+      <c r="O13" s="32">
+        <f t="shared" ref="O13" si="6">AVERAGE(N13/12)</f>
+        <v>3201.1666666666665</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="33"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="11"/>
+      <c r="B14" s="32">
+        <f>AVERAGE(B9:B12)</f>
+        <v>1097</v>
+      </c>
+      <c r="C14" s="32">
+        <f t="shared" ref="C14:N14" si="7">AVERAGE(C9:C12)</f>
+        <v>931</v>
+      </c>
+      <c r="D14" s="32">
+        <f t="shared" si="7"/>
+        <v>1330.3333333333333</v>
+      </c>
+      <c r="E14" s="32">
+        <f t="shared" si="7"/>
+        <v>1126</v>
+      </c>
+      <c r="F14" s="32">
+        <f t="shared" si="7"/>
+        <v>1013</v>
+      </c>
+      <c r="G14" s="32">
+        <f t="shared" si="7"/>
+        <v>996</v>
+      </c>
+      <c r="H14" s="32">
+        <f t="shared" si="7"/>
+        <v>1177.6666666666667</v>
+      </c>
+      <c r="I14" s="32">
+        <f t="shared" si="7"/>
+        <v>1050</v>
+      </c>
+      <c r="J14" s="32">
+        <f t="shared" si="7"/>
+        <v>997.66666666666663</v>
+      </c>
+      <c r="K14" s="32">
+        <f t="shared" si="7"/>
+        <v>1013.6666666666666</v>
+      </c>
+      <c r="L14" s="32">
+        <f>AVERAGE(L9:L12)</f>
+        <v>842.66666666666663</v>
+      </c>
+      <c r="M14" s="32">
+        <f t="shared" si="7"/>
+        <v>1229.6666666666667</v>
+      </c>
+      <c r="N14" s="32">
+        <f t="shared" si="7"/>
+        <v>12804.666666666666</v>
+      </c>
+      <c r="O14" s="32">
+        <f>AVERAGE(O9:O12)</f>
+        <v>1067.0555555555557</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
@@ -6790,6 +6944,7 @@
       <c r="O19" s="11"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
       <c r="B20" s="30"/>
       <c r="C20" s="30"/>
       <c r="D20" s="30"/>
@@ -6806,7 +6961,6 @@
       <c r="O20" s="11"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
       <c r="B21" s="30"/>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
@@ -6824,19 +6978,19 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
       <c r="O22" s="11"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -6850,7 +7004,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
+      <c r="K23" s="33"/>
       <c r="L23" s="11"/>
       <c r="M23" s="11"/>
       <c r="N23" s="11"/>
@@ -6874,15 +7028,21 @@
       <c r="O24" s="11"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
@@ -6893,17 +7053,18 @@
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
-      <c r="I26" s="14"/>
+      <c r="I26" s="12"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="14"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
@@ -7215,9 +7376,23 @@
       <c r="G58" s="18"/>
       <c r="H58" s="18"/>
     </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="18"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="B4:C4"/>
@@ -7227,9 +7402,9 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
   </mergeCells>
-  <conditionalFormatting sqref="H11">
+  <conditionalFormatting sqref="H12">
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Vencida">
-      <formula>NOT(ISERROR(SEARCH("Vencida",H11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Vencida",H12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>